<commit_message>
update template excel pembayaran
</commit_message>
<xml_diff>
--- a/uploads/finance/TemplatePembayaran.xlsx
+++ b/uploads/finance/TemplatePembayaran.xlsx
@@ -63,9 +63,6 @@
     <t>NIM</t>
   </si>
   <si>
-    <t>WINNIE SAVIRA</t>
-  </si>
-  <si>
     <t>Akuntansi</t>
   </si>
   <si>
@@ -76,6 +73,9 @@
   </si>
   <si>
     <t>Ketarangan</t>
+  </si>
+  <si>
+    <t>WINNIE SAVIRA1</t>
   </si>
 </sst>
 </file>
@@ -625,7 +625,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -648,7 +648,7 @@
     </row>
     <row r="2" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -700,7 +700,7 @@
         <v>9</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I6" s="11" t="s">
         <v>10</v>
@@ -715,13 +715,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C7" s="13">
         <v>12170001</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="7"/>
@@ -740,13 +740,13 @@
         <v>2</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="13">
         <v>12170002</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="7"/>

</xml_diff>

<commit_message>
update penerimaan pembayaran mhs
</commit_message>
<xml_diff>
--- a/uploads/finance/TemplatePembayaran.xlsx
+++ b/uploads/finance/TemplatePembayaran.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\puis\uploads\finance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Podomoro University\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="270" yWindow="90" windowWidth="11040" windowHeight="7605"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$D$5:$D$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$6</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -25,11 +24,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>YAYASAN PENDIDIKAN AGUNG PODOMORO</t>
   </si>
   <si>
+    <t>Rekap Penerimaan &amp; AGING 2018/2019 Ganjil</t>
+  </si>
+  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -39,6 +41,9 @@
     <t>NAMA</t>
   </si>
   <si>
+    <t>NIM</t>
+  </si>
+  <si>
     <t>JURUSAN</t>
   </si>
   <si>
@@ -60,71 +65,89 @@
     <t>SKS</t>
   </si>
   <si>
-    <t>NIM</t>
-  </si>
-  <si>
-    <t>REKAP PENERIMAAN &amp; AGING 2016/2017 Gasal (SEMESTER 2)</t>
-  </si>
-  <si>
-    <t>Ketarangan</t>
+    <t>DEOGA PRAYUDHA</t>
+  </si>
+  <si>
+    <t>Accounting</t>
+  </si>
+  <si>
+    <t>Lunas</t>
+  </si>
+  <si>
+    <t>MUHAMMAD KAHFI JUSUP</t>
+  </si>
+  <si>
+    <t>Entrepreneurship</t>
+  </si>
+  <si>
+    <t>Demo User ARC</t>
+  </si>
+  <si>
+    <t>Architecture</t>
+  </si>
+  <si>
+    <t>Jumlah</t>
+  </si>
+  <si>
+    <t>Ket</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2FE1F9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -134,55 +157,55 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -190,88 +213,102 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="17">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="Comma 2" xfId="2"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 4" xfId="4"/>
-    <cellStyle name="Normal 5" xfId="3"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF2FE1F9"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -326,7 +363,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -361,7 +398,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -570,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -586,7 +623,7 @@
     <col min="6" max="8" width="14" style="1" customWidth="1"/>
     <col min="9" max="10" width="14.140625" style="1" customWidth="1"/>
     <col min="11" max="11" width="41" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="12" max="12" width="9.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -596,84 +633,177 @@
     </row>
     <row r="2" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="D3" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
     </row>
     <row r="5" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="15"/>
+      <c r="I6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="15"/>
+      <c r="K6" s="12"/>
+    </row>
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="13"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>1</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="6">
+        <v>12150001</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7">
+        <v>8400000</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+    </row>
+    <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
         <v>2</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="6">
+        <v>11140031</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7">
+        <v>14000000</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
         <v>3</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="K6" s="8"/>
+      <c r="B10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="6">
+        <v>21180001</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7">
+        <v>8000000</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
     </row>
   </sheetData>
-  <sortState ref="B8:S202">
-    <sortCondition ref="D8:D202"/>
-    <sortCondition ref="C8:C202"/>
-  </sortState>
-  <mergeCells count="6">
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="D5:D6"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <mergeCells count="10">
     <mergeCell ref="E5:J5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K5:K7"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="1" bottom="0" header="0" footer="0"/>
-  <pageSetup scale="41" orientation="landscape" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup scale="41" orientation="landscape"/>
 </worksheet>
 </file>
 
@@ -685,6 +815,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -697,6 +828,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>